<commit_message>
upload new code from Nam
</commit_message>
<xml_diff>
--- a/datas/Option_B/Datas_cleaned/FINAL CONSUMPTION_Brazil.xlsx
+++ b/datas/Option_B/Datas_cleaned/FINAL CONSUMPTION_Brazil.xlsx
@@ -1,37 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>TOTAL PRIMARIES</t>
+  </si>
+  <si>
+    <t>TOTAL SECUNDARIES</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +66,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,911 +382,756 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>TOTAL PRIMARIES</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>TOTAL SECUNDARIES</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>NON-ENERGY</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
         <v>1970</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>31635.21</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>27198.9</v>
       </c>
-      <c r="D2" t="n">
-        <v>1201.77</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="D2">
         <v>58834.12</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
         <v>1971</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>31374.67</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>30317.01</v>
       </c>
-      <c r="D3" t="n">
-        <v>1173.62</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="D3">
         <v>61691.69</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
         <v>1972</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>31596.5</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>34398.62</v>
       </c>
-      <c r="D4" t="n">
-        <v>1238.57</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="D4">
         <v>65995.12</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
         <v>1973</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>31403.26</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>40289.6</v>
       </c>
-      <c r="D5" t="n">
-        <v>1238.57</v>
-      </c>
-      <c r="E5" t="n">
+      <c r="D5">
         <v>71692.86</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
         <v>1974</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>31085.05</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>45113.35</v>
       </c>
-      <c r="D6" t="n">
-        <v>2002.12</v>
-      </c>
-      <c r="E6" t="n">
+      <c r="D6">
         <v>76198.39999999999</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
         <v>1975</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>30053.88</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>48437.97</v>
       </c>
-      <c r="D7" t="n">
-        <v>2118.99</v>
-      </c>
-      <c r="E7" t="n">
+      <c r="D7">
         <v>78491.85000000001</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
         <v>1976</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>30083.43</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>53125.54</v>
       </c>
-      <c r="D8" t="n">
-        <v>2267.92</v>
-      </c>
-      <c r="E8" t="n">
+      <c r="D8">
         <v>83208.97</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
         <v>1977</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>29984.29</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>55042.22</v>
       </c>
-      <c r="D9" t="n">
-        <v>2457.26</v>
-      </c>
-      <c r="E9" t="n">
+      <c r="D9">
         <v>85026.52</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
         <v>1978</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>28615.38</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>60329.58</v>
       </c>
-      <c r="D10" t="n">
-        <v>2976.05</v>
-      </c>
-      <c r="E10" t="n">
+      <c r="D10">
         <v>88944.97</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
         <v>1979</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>28029.19</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>65752.89999999999</v>
       </c>
-      <c r="D11" t="n">
-        <v>3786.66</v>
-      </c>
-      <c r="E11" t="n">
+      <c r="D11">
         <v>93782.10000000001</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
         <v>1980</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>28638.89</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>65895.95</v>
       </c>
-      <c r="D12" t="n">
-        <v>3181.99</v>
-      </c>
-      <c r="E12" t="n">
+      <c r="D12">
         <v>94534.85000000001</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
         <v>1981</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>28970.26</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>62262.56</v>
       </c>
-      <c r="D13" t="n">
-        <v>2718.84</v>
-      </c>
-      <c r="E13" t="n">
+      <c r="D13">
         <v>91232.82000000001</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
         <v>1982</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>28301.57</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14">
         <v>64160.85</v>
       </c>
-      <c r="D14" t="n">
-        <v>2934.74</v>
-      </c>
-      <c r="E14" t="n">
+      <c r="D14">
         <v>92462.42</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
         <v>1983</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>29173.95</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>63026.78</v>
       </c>
-      <c r="D15" t="n">
-        <v>2505.53</v>
-      </c>
-      <c r="E15" t="n">
+      <c r="D15">
         <v>92200.73</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
         <v>1984</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>29912.45</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
         <v>65309.87</v>
       </c>
-      <c r="D16" t="n">
-        <v>2617.73</v>
-      </c>
-      <c r="E16" t="n">
+      <c r="D16">
         <v>95222.32000000001</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
         <v>1985</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>29045.82</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17">
         <v>70588.89999999999</v>
       </c>
-      <c r="D17" t="n">
-        <v>3370.18</v>
-      </c>
-      <c r="E17" t="n">
+      <c r="D17">
         <v>99634.71000000001</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
         <v>1986</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>28706.5</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18">
         <v>76544.78999999999</v>
       </c>
-      <c r="D18" t="n">
-        <v>3061.72</v>
-      </c>
-      <c r="E18" t="n">
+      <c r="D18">
         <v>105251.29</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
         <v>1987</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>30039.49</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19">
         <v>78768.2</v>
       </c>
-      <c r="D19" t="n">
-        <v>3015.71</v>
-      </c>
-      <c r="E19" t="n">
+      <c r="D19">
         <v>108807.69</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
         <v>1988</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>28430.03</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20">
         <v>81326.64999999999</v>
       </c>
-      <c r="D20" t="n">
-        <v>3101.27</v>
-      </c>
-      <c r="E20" t="n">
+      <c r="D20">
         <v>109756.68</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
         <v>1989</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>26448.78</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21">
         <v>85037.8</v>
       </c>
-      <c r="D21" t="n">
-        <v>3015.47</v>
-      </c>
-      <c r="E21" t="n">
+      <c r="D21">
         <v>111486.58</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
         <v>1990</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>28088.2</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22">
         <v>86262.86</v>
       </c>
-      <c r="D22" t="n">
-        <v>3232.54</v>
-      </c>
-      <c r="E22" t="n">
+      <c r="D22">
         <v>114351.06</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
         <v>1991</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>28470.83</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23">
         <v>87004.27</v>
       </c>
-      <c r="D23" t="n">
-        <v>2998.38</v>
-      </c>
-      <c r="E23" t="n">
+      <c r="D23">
         <v>115475.1</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
         <v>1992</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>28621.02</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24">
         <v>88235.25999999999</v>
       </c>
-      <c r="D24" t="n">
-        <v>2956.49</v>
-      </c>
-      <c r="E24" t="n">
+      <c r="D24">
         <v>116856.28</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:4">
+      <c r="A25" s="1">
         <v>1993</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>28001.03</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25">
         <v>92001.64999999999</v>
       </c>
-      <c r="D25" t="n">
-        <v>2945.9</v>
-      </c>
-      <c r="E25" t="n">
+      <c r="D25">
         <v>120002.68</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:4">
+      <c r="A26" s="1">
         <v>1994</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>29792.29</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26">
         <v>96468.44</v>
       </c>
-      <c r="D26" t="n">
-        <v>3151.72</v>
-      </c>
-      <c r="E26" t="n">
+      <c r="D26">
         <v>126260.73</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:4">
+      <c r="A27" s="1">
         <v>1995</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>29434.73</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27">
         <v>102081.6</v>
       </c>
-      <c r="D27" t="n">
-        <v>3006.77</v>
-      </c>
-      <c r="E27" t="n">
+      <c r="D27">
         <v>131516.33</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
+    <row r="28" spans="1:4">
+      <c r="A28" s="1">
         <v>1996</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>30629</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28">
         <v>107582.73</v>
       </c>
-      <c r="D28" t="n">
-        <v>3396.1</v>
-      </c>
-      <c r="E28" t="n">
+      <c r="D28">
         <v>138211.73</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
+    <row r="29" spans="1:4">
+      <c r="A29" s="1">
         <v>1997</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29">
         <v>29330.32</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29">
         <v>113774.52</v>
       </c>
-      <c r="D29" t="n">
-        <v>3745.85</v>
-      </c>
-      <c r="E29" t="n">
+      <c r="D29">
         <v>143104.84</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
+    <row r="30" spans="1:4">
+      <c r="A30" s="1">
         <v>1998</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>31041</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30">
         <v>116944.32</v>
       </c>
-      <c r="D30" t="n">
-        <v>4222.88</v>
-      </c>
-      <c r="E30" t="n">
+      <c r="D30">
         <v>147985.31</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
+    <row r="31" spans="1:4">
+      <c r="A31" s="1">
         <v>1999</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>36297.47</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31">
         <v>118924.51</v>
       </c>
-      <c r="D31" t="n">
-        <v>4102.58</v>
-      </c>
-      <c r="E31" t="n">
+      <c r="D31">
         <v>155221.98</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
+    <row r="32" spans="1:4">
+      <c r="A32" s="1">
         <v>2000</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>35893.32</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32">
         <v>120915.27</v>
       </c>
-      <c r="D32" t="n">
-        <v>4447.39</v>
-      </c>
-      <c r="E32" t="n">
+      <c r="D32">
         <v>156808.59</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
         <v>2001</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>38866.8</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33">
         <v>117648.5</v>
       </c>
-      <c r="D33" t="n">
-        <v>3876.42</v>
-      </c>
-      <c r="E33" t="n">
+      <c r="D33">
         <v>156515.3</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
         <v>2002</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>39586.34</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34">
         <v>120091.8</v>
       </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="n">
+      <c r="D34">
         <v>159678.14</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
         <v>2003</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>42350.37</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35">
         <v>119009.34</v>
       </c>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="n">
+      <c r="D35">
         <v>161359.72</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
         <v>2004</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36">
         <v>45339.22</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36">
         <v>124959.48</v>
       </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="n">
+      <c r="D36">
         <v>170298.7</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
         <v>2005</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37">
         <v>46911.29</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C37">
         <v>126194.57</v>
       </c>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="n">
+      <c r="D37">
         <v>173105.86</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
         <v>2006</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38">
         <v>50549.71</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38">
         <v>127727.03</v>
       </c>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="n">
+      <c r="D38">
         <v>178276.74</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
         <v>2007</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39">
         <v>52784.82</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39">
         <v>136356.06</v>
       </c>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="n">
+      <c r="D39">
         <v>189140.88</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="1" t="n">
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
         <v>2008</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40">
         <v>53033.86</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C40">
         <v>142379.08</v>
       </c>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="n">
+      <c r="D40">
         <v>195412.94</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="1" t="n">
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
         <v>2009</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41">
         <v>51574.68</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C41">
         <v>139240.15</v>
       </c>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="n">
+      <c r="D41">
         <v>190814.83</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="1" t="n">
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
         <v>2010</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42">
         <v>56568.67</v>
       </c>
-      <c r="C42" t="n">
+      <c r="C42">
         <v>151143.82</v>
       </c>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="n">
+      <c r="D42">
         <v>207712.48</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="1" t="n">
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
         <v>2011</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43">
         <v>56213.76</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C43">
         <v>158645.77</v>
       </c>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="n">
+      <c r="D43">
         <v>214859.53</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="1" t="n">
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
         <v>2012</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44">
         <v>56806.08</v>
       </c>
-      <c r="C44" t="n">
+      <c r="C44">
         <v>172968</v>
       </c>
-      <c r="D44" t="n">
-        <v>7516.16</v>
-      </c>
-      <c r="E44" t="n">
+      <c r="D44">
         <v>229774.08</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="1" t="n">
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
         <v>2013</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45">
         <v>56121.57</v>
       </c>
-      <c r="C45" t="n">
+      <c r="C45">
         <v>177591.67</v>
       </c>
-      <c r="D45" t="n">
-        <v>7800.96</v>
-      </c>
-      <c r="E45" t="n">
+      <c r="D45">
         <v>233713.25</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="1" t="n">
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
         <v>2014</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46">
         <v>55830.06</v>
       </c>
-      <c r="C46" t="n">
+      <c r="C46">
         <v>181933.07</v>
       </c>
-      <c r="D46" t="n">
-        <v>8102.65</v>
-      </c>
-      <c r="E46" t="n">
+      <c r="D46">
         <v>237763.12</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="1" t="n">
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
         <v>2015</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47">
         <v>55641.51</v>
       </c>
-      <c r="C47" t="n">
+      <c r="C47">
         <v>176895.55</v>
       </c>
-      <c r="D47" t="n">
-        <v>6737.28</v>
-      </c>
-      <c r="E47" t="n">
+      <c r="D47">
         <v>232537.06</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="1" t="n">
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
         <v>2016</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48">
         <v>55834.06</v>
       </c>
-      <c r="C48" t="n">
+      <c r="C48">
         <v>172818.98</v>
       </c>
-      <c r="D48" t="n">
-        <v>6923.39</v>
-      </c>
-      <c r="E48" t="n">
+      <c r="D48">
         <v>228653.04</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="1" t="n">
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
         <v>2017</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49">
         <v>57433.64</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C49">
         <v>175570.99</v>
       </c>
-      <c r="D49" t="n">
-        <v>6313.17</v>
-      </c>
-      <c r="E49" t="n">
+      <c r="D49">
         <v>233004.63</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
         <v>2018</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50">
         <v>55123.82</v>
       </c>
-      <c r="C50" t="n">
+      <c r="C50">
         <v>173541.56</v>
       </c>
-      <c r="D50" t="n">
-        <v>6344.02</v>
-      </c>
-      <c r="E50" t="n">
+      <c r="D50">
         <v>228665.38</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
         <v>2019</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51">
         <v>53183.55</v>
       </c>
-      <c r="C51" t="n">
+      <c r="C51">
         <v>177114.5</v>
       </c>
-      <c r="D51" t="n">
-        <v>6477.42</v>
-      </c>
-      <c r="E51" t="n">
+      <c r="D51">
         <v>230298.05</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
         <v>2020</v>
       </c>
-      <c r="B52" t="n">
+      <c r="B52">
         <v>57568.22</v>
       </c>
-      <c r="C52" t="n">
+      <c r="C52">
         <v>169391.55</v>
       </c>
-      <c r="D52" t="n">
-        <v>6875</v>
-      </c>
-      <c r="E52" t="n">
+      <c r="D52">
         <v>226959.77</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="1" t="n">
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
         <v>2021</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53">
         <v>58156.56</v>
       </c>
-      <c r="C53" t="n">
+      <c r="C53">
         <v>179037.96</v>
       </c>
-      <c r="D53" t="n">
-        <v>6626.69</v>
-      </c>
-      <c r="E53" t="n">
+      <c r="D53">
         <v>237194.52</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>